<commit_message>
Links to GitHub STL added
</commit_message>
<xml_diff>
--- a/bom/BOM_WaterCooling_Bay.xlsx
+++ b/bom/BOM_WaterCooling_Bay.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8bf86f88c49aa82/Documents/GitHub/HevORT/bom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{FA6671E9-AAFF-4543-8BEF-236E95709AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC564C8C-3AC1-4DF2-86FA-AD15B2EC7C30}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{FA6671E9-AAFF-4543-8BEF-236E95709AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{779CF2A4-FCF1-46EA-9BF2-460BCCDCB7C9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="103">
   <si>
     <t>Thumbnail</t>
   </si>
@@ -371,6 +371,30 @@
   </si>
   <si>
     <t>Length is equivalent to your frame Horizontal Back and Horizontal Front 3030 extrusion + 60mm</t>
+  </si>
+  <si>
+    <t>https://github.com/MirageC79/HevORT/blob/master/files/STL/Enclosure/WaterCooling_Bay/Cooling%20Spider%20Base.stl</t>
+  </si>
+  <si>
+    <t>https://github.com/MirageC79/HevORT/blob/master/files/STL/Enclosure/WaterCooling_Bay/Mounting_Spacer.stl</t>
+  </si>
+  <si>
+    <t>https://github.com/MirageC79/HevORT/blob/master/files/STL/Enclosure/WaterCooling_Bay/WaterPumpBracket.stl</t>
+  </si>
+  <si>
+    <t>https://github.com/MirageC79/HevORT/blob/master/files/STL/Enclosure/WaterCooling_Bay/WaterCoolingTray_Support.stl</t>
+  </si>
+  <si>
+    <t>https://github.com/MirageC79/HevORT/blob/master/files/STL/Enclosure/WaterCooling_Bay/WaterCoolingTray_Support_Top_LH.stl</t>
+  </si>
+  <si>
+    <t>https://github.com/MirageC79/HevORT/blob/master/files/STL/Enclosure/WaterCooling_Bay/WaterCoolingTray_Support_Top_RH.stl</t>
+  </si>
+  <si>
+    <t>https://github.com/MirageC79/HevORT/blob/master/files/STL/Enclosure/WaterCooling_Bay/WaterCoolingBay_BracketClipRH.stl</t>
+  </si>
+  <si>
+    <t>https://github.com/MirageC79/HevORT/blob/master/files/STL/Enclosure/WaterCooling_Bay/WaterCoolingBay_BracketClipLH.stl</t>
   </si>
 </sst>
 </file>
@@ -587,9 +611,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -640,6 +661,9 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1057,6 +1081,20 @@
         <horizontal style="thin">
           <color theme="6" tint="-0.249977111117893"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FFFFFF00"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FFFFFF00"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1092,20 +1130,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FFFFFF00"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color rgb="FFFFFF00"/>
-        </top>
       </border>
     </dxf>
   </dxfs>
@@ -2618,7 +2642,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5B5A722D-C4EF-4D88-A7A2-FF0AA6DF9209}" name="Table1" displayName="Table1" ref="A2:K32" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5B5A722D-C4EF-4D88-A7A2-FF0AA6DF9209}" name="Table1" displayName="Table1" ref="A2:K32" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11">
   <autoFilter ref="A2:K32" xr:uid="{5B5A722D-C4EF-4D88-A7A2-FF0AA6DF9209}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:K29">
     <sortCondition ref="B2:B29"/>
@@ -2929,9 +2953,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2946,964 +2968,984 @@
     <col min="11" max="11" width="48.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="7" customFormat="1" ht="248.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="6" customFormat="1" ht="248.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
-      <c r="E1" s="22" t="str">
+      <c r="E1" s="21" t="str">
         <f>HYPERLINK("https://a360.co/3PBfjxU","LINK TO CAD")</f>
         <v>LINK TO CAD</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
     </row>
-    <row r="2" spans="1:11" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:11" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="17" t="s">
+      <c r="D3" s="15"/>
+      <c r="E3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="14">
         <v>2</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="19" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="17" t="s">
+      <c r="D4" s="15"/>
+      <c r="E4" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="14">
         <v>6</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="I4" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="20" t="s">
+      <c r="K4" s="19" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="17" t="s">
+      <c r="D5" s="15"/>
+      <c r="E5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="14">
         <v>6</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="I5" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="20" t="s">
+      <c r="K5" s="19" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="17" t="s">
+      <c r="D6" s="15"/>
+      <c r="E6" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="J6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="20" t="s">
+      <c r="K6" s="19" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="17" t="s">
+      <c r="D7" s="15"/>
+      <c r="E7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="J7" s="19"/>
-      <c r="K7" s="21"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="20"/>
     </row>
     <row r="8" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="14">
         <v>6</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="17" t="s">
+      <c r="D8" s="15"/>
+      <c r="E8" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="14">
         <v>8</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="20" t="s">
+      <c r="K8" s="19" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="14">
         <v>7</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="17" t="s">
+      <c r="D9" s="15"/>
+      <c r="E9" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="14">
         <v>4</v>
       </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="21"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="20"/>
     </row>
     <row r="10" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="14">
         <v>8</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="17" t="s">
+      <c r="D10" s="15"/>
+      <c r="E10" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="14">
         <v>4</v>
       </c>
-      <c r="I10" s="18"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="21"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="20"/>
     </row>
     <row r="11" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="14">
         <v>9</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="17" t="s">
+      <c r="D11" s="15"/>
+      <c r="E11" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="14">
         <v>3</v>
       </c>
-      <c r="I11" s="18"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="21"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="20"/>
     </row>
     <row r="12" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="14">
         <v>10</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="17" t="s">
+      <c r="D12" s="15"/>
+      <c r="E12" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="15" t="s">
+      <c r="F12" s="16"/>
+      <c r="G12" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="14">
         <v>21</v>
       </c>
-      <c r="I12" s="18"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="21"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="20"/>
     </row>
     <row r="13" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="14">
         <v>11</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="17" t="s">
+      <c r="D13" s="15"/>
+      <c r="E13" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="15" t="s">
+      <c r="F13" s="16"/>
+      <c r="G13" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="14">
         <v>18</v>
       </c>
-      <c r="I13" s="18"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="21"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="20"/>
     </row>
     <row r="14" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="14">
         <v>12</v>
       </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="17" t="s">
+      <c r="D14" s="15"/>
+      <c r="E14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H14" s="14">
         <v>30</v>
       </c>
-      <c r="I14" s="18"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="21"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="20"/>
     </row>
     <row r="15" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="14">
         <v>13</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="17" t="s">
+      <c r="D15" s="15"/>
+      <c r="E15" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="G15" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="14">
         <v>28</v>
       </c>
-      <c r="I15" s="18"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="21"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="20"/>
     </row>
     <row r="16" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="14">
         <v>14</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="17" t="s">
+      <c r="D16" s="15"/>
+      <c r="E16" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="17"/>
-      <c r="G16" s="15" t="s">
+      <c r="F16" s="16"/>
+      <c r="G16" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="15">
+      <c r="H16" s="14">
         <v>3</v>
       </c>
-      <c r="I16" s="18" t="s">
+      <c r="I16" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="J16" s="19"/>
-      <c r="K16" s="21"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="20"/>
     </row>
     <row r="17" spans="1:11" ht="165" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="14">
         <v>15</v>
       </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="17" t="s">
+      <c r="D17" s="15"/>
+      <c r="E17" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="G17" s="15" t="s">
+      <c r="G17" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="15">
+      <c r="H17" s="14">
         <v>1</v>
       </c>
-      <c r="I17" s="18" t="s">
+      <c r="I17" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="J17" s="19" t="s">
+      <c r="J17" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="K17" s="20" t="s">
+      <c r="K17" s="19" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="14">
         <v>16</v>
       </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="17" t="s">
+      <c r="D18" s="15"/>
+      <c r="E18" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="F18" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="G18" s="15" t="s">
+      <c r="G18" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H18" s="15">
+      <c r="H18" s="14">
         <v>2</v>
       </c>
-      <c r="I18" s="18" t="s">
+      <c r="I18" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="J18" s="19" t="s">
+      <c r="J18" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="K18" s="20" t="s">
+      <c r="K18" s="19" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="14">
         <v>17</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="17" t="s">
+      <c r="D19" s="15"/>
+      <c r="E19" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="G19" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="15">
+      <c r="H19" s="14">
         <v>8</v>
       </c>
-      <c r="I19" s="18" t="s">
+      <c r="I19" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="J19" s="19"/>
-      <c r="K19" s="21"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="20"/>
     </row>
     <row r="20" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="14">
         <v>18</v>
       </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="17" t="s">
+      <c r="D20" s="15"/>
+      <c r="E20" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="17" t="s">
+      <c r="F20" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H20" s="15">
+      <c r="H20" s="14">
         <v>8</v>
       </c>
-      <c r="I20" s="18" t="s">
+      <c r="I20" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="J20" s="19"/>
-      <c r="K20" s="21"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="20"/>
     </row>
     <row r="21" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21" s="14">
         <v>19</v>
       </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="17" t="s">
+      <c r="D21" s="15"/>
+      <c r="E21" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="F21" s="17" t="s">
+      <c r="F21" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="G21" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H21" s="15">
+      <c r="H21" s="14">
         <v>1</v>
       </c>
-      <c r="I21" s="18" t="s">
+      <c r="I21" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="J21" s="19"/>
-      <c r="K21" s="21"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="20"/>
     </row>
     <row r="22" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C22" s="14">
         <v>20</v>
       </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="17" t="s">
+      <c r="D22" s="15"/>
+      <c r="E22" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="17"/>
-      <c r="G22" s="15" t="s">
+      <c r="F22" s="16"/>
+      <c r="G22" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H22" s="15">
+      <c r="H22" s="14">
         <v>1</v>
       </c>
-      <c r="I22" s="18" t="s">
+      <c r="I22" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="J22" s="19"/>
-      <c r="K22" s="21"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="19" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="23" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C23" s="14">
         <v>21</v>
       </c>
-      <c r="D23" s="16"/>
-      <c r="E23" s="17" t="s">
+      <c r="D23" s="15"/>
+      <c r="E23" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="17"/>
-      <c r="G23" s="15" t="s">
+      <c r="F23" s="16"/>
+      <c r="G23" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H23" s="15">
+      <c r="H23" s="14">
         <v>1</v>
       </c>
-      <c r="I23" s="18"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="21"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="19" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="24" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="15">
+      <c r="C24" s="14">
         <v>22</v>
       </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="17" t="s">
+      <c r="D24" s="15"/>
+      <c r="E24" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="17"/>
-      <c r="G24" s="15" t="s">
+      <c r="F24" s="16"/>
+      <c r="G24" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H24" s="15">
+      <c r="H24" s="14">
         <v>1</v>
       </c>
-      <c r="I24" s="18" t="s">
+      <c r="I24" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="J24" s="19" t="s">
+      <c r="J24" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="K24" s="20" t="s">
+      <c r="K24" s="19" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C25" s="14">
         <v>23</v>
       </c>
-      <c r="D25" s="16"/>
-      <c r="E25" s="17" t="s">
+      <c r="D25" s="15"/>
+      <c r="E25" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F25" s="17"/>
-      <c r="G25" s="15" t="s">
+      <c r="F25" s="16"/>
+      <c r="G25" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H25" s="15">
+      <c r="H25" s="14">
         <v>2</v>
       </c>
-      <c r="I25" s="18" t="s">
+      <c r="I25" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="J25" s="19" t="s">
+      <c r="J25" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="K25" s="20" t="s">
+      <c r="K25" s="19" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C26" s="14">
         <v>24</v>
       </c>
-      <c r="D26" s="16"/>
-      <c r="E26" s="17" t="s">
+      <c r="D26" s="15"/>
+      <c r="E26" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F26" s="17"/>
-      <c r="G26" s="15" t="s">
+      <c r="F26" s="16"/>
+      <c r="G26" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H26" s="15">
+      <c r="H26" s="14">
         <v>1</v>
       </c>
-      <c r="I26" s="18" t="s">
+      <c r="I26" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="J26" s="19" t="s">
+      <c r="J26" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="K26" s="20" t="s">
+      <c r="K26" s="19" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27" s="14">
         <v>27</v>
       </c>
-      <c r="D27" s="16"/>
-      <c r="E27" s="17" t="s">
+      <c r="D27" s="15"/>
+      <c r="E27" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="17"/>
-      <c r="G27" s="15" t="s">
+      <c r="F27" s="16"/>
+      <c r="G27" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H27" s="15">
+      <c r="H27" s="14">
         <v>1</v>
       </c>
-      <c r="I27" s="18"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="21"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="19" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="28" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="15">
+      <c r="C28" s="14">
         <v>28</v>
       </c>
-      <c r="D28" s="16"/>
-      <c r="E28" s="17" t="s">
+      <c r="D28" s="15"/>
+      <c r="E28" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="F28" s="17"/>
-      <c r="G28" s="15" t="s">
+      <c r="F28" s="16"/>
+      <c r="G28" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H28" s="15">
+      <c r="H28" s="14">
         <v>1</v>
       </c>
-      <c r="I28" s="18" t="s">
+      <c r="I28" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="J28" s="19"/>
-      <c r="K28" s="21"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="19" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="29" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="15">
+      <c r="C29" s="14">
         <v>29</v>
       </c>
-      <c r="D29" s="16"/>
-      <c r="E29" s="17" t="s">
+      <c r="D29" s="15"/>
+      <c r="E29" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="F29" s="17"/>
-      <c r="G29" s="15" t="s">
+      <c r="F29" s="16"/>
+      <c r="G29" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H29" s="15">
+      <c r="H29" s="14">
         <v>4</v>
       </c>
-      <c r="I29" s="18"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="21"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="19" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="30" spans="1:11" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="15">
+      <c r="C30" s="14">
         <v>30</v>
       </c>
-      <c r="D30" s="16"/>
-      <c r="E30" s="17" t="s">
+      <c r="D30" s="15"/>
+      <c r="E30" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="F30" s="17"/>
-      <c r="G30" s="15" t="s">
+      <c r="F30" s="16"/>
+      <c r="G30" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H30" s="15">
+      <c r="H30" s="14">
         <v>4</v>
       </c>
-      <c r="I30" s="18"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="21"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="19" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="31" spans="1:11" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="15">
+      <c r="C31" s="14">
         <v>31</v>
       </c>
-      <c r="D31" s="16"/>
-      <c r="E31" s="17" t="s">
+      <c r="D31" s="15"/>
+      <c r="E31" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="F31" s="17"/>
-      <c r="G31" s="15" t="s">
+      <c r="F31" s="16"/>
+      <c r="G31" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H31" s="15">
+      <c r="H31" s="14">
         <v>1</v>
       </c>
-      <c r="I31" s="18"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="21"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="19" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="32" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C32" s="15">
+      <c r="C32" s="14">
         <v>26</v>
       </c>
-      <c r="D32" s="16"/>
-      <c r="E32" s="17" t="s">
+      <c r="D32" s="15"/>
+      <c r="E32" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="F32" s="17"/>
-      <c r="G32" s="15" t="s">
+      <c r="F32" s="16"/>
+      <c r="G32" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H32" s="15">
+      <c r="H32" s="14">
         <v>1</v>
       </c>
-      <c r="I32" s="18"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="21"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="19" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="33" spans="1:11" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="15">
+      <c r="C33" s="14">
         <v>32</v>
       </c>
-      <c r="D33" s="16"/>
-      <c r="E33" s="17" t="s">
+      <c r="D33" s="15"/>
+      <c r="E33" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="F33" s="17"/>
-      <c r="G33" s="15" t="s">
+      <c r="F33" s="16"/>
+      <c r="G33" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H33" s="15">
+      <c r="H33" s="14">
         <v>1</v>
       </c>
-      <c r="I33" s="18"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="21"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="19" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="34" spans="1:11" ht="126" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="15">
+      <c r="C34" s="14">
         <v>25</v>
       </c>
-      <c r="D34" s="16"/>
-      <c r="E34" s="17" t="s">
+      <c r="D34" s="15"/>
+      <c r="E34" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="F34" s="17"/>
-      <c r="G34" s="15" t="s">
+      <c r="F34" s="16"/>
+      <c r="G34" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H34" s="15">
+      <c r="H34" s="14">
         <v>1</v>
       </c>
-      <c r="I34" s="18"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="21"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="19" t="s">
+        <v>102</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3920,14 +3962,24 @@
     <hyperlink ref="K24" r:id="rId8" xr:uid="{5531BAE6-2ABA-479C-A4A4-20CF4F8E2DE6}"/>
     <hyperlink ref="K25" r:id="rId9" xr:uid="{12AF442A-1A01-45A4-87E6-167B376163E9}"/>
     <hyperlink ref="K26" r:id="rId10" xr:uid="{60B1F400-EE70-4F40-8DBA-1C425F3D0417}"/>
+    <hyperlink ref="K22" r:id="rId11" xr:uid="{1101F55A-C9CE-44C2-8796-475B2E59ED59}"/>
+    <hyperlink ref="K23" r:id="rId12" xr:uid="{FA0B7E0B-796B-4CF0-87FD-C00525E2916E}"/>
+    <hyperlink ref="K27" r:id="rId13" xr:uid="{2FA85849-599B-4870-AC5D-753BFBC6A21D}"/>
+    <hyperlink ref="K28" r:id="rId14" xr:uid="{B64E6D0F-61DD-4490-8BA8-112F30540933}"/>
+    <hyperlink ref="K29" r:id="rId15" xr:uid="{D69268A2-E31E-4387-B600-F30C60609768}"/>
+    <hyperlink ref="K31" r:id="rId16" xr:uid="{7076B76C-E66B-4A18-BAFF-868DB95AEAA8}"/>
+    <hyperlink ref="K32" r:id="rId17" xr:uid="{61E132EB-EBDC-49C7-AD01-7637C709B9C8}"/>
+    <hyperlink ref="K34" r:id="rId18" xr:uid="{C03597CC-A7DC-49C1-B083-2277644EEB63}"/>
+    <hyperlink ref="K33" r:id="rId19" xr:uid="{E7EA8D60-9DDA-40D8-A6B3-93B774456E30}"/>
+    <hyperlink ref="K30" r:id="rId20" xr:uid="{54316BB2-F438-4DFC-9B8A-67883B52A4F7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId11"/>
+  <drawing r:id="rId21"/>
   <webPublishItems count="1">
     <webPublishItem id="23836" divId="BOM_WaterCooling_Bay_23836" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\BOM_WaterCooling_Bay.htm" autoRepublish="1"/>
   </webPublishItems>
   <tableParts count="1">
-    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId22"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>